<commit_message>
new post who dis
</commit_message>
<xml_diff>
--- a/content/page/data.xlsx
+++ b/content/page/data.xlsx
@@ -14,6 +14,39 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="90">
   <si>
+    <t>skill</t>
+  </si>
+  <si>
+    <t>Data Science</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Business Intelligence</t>
+  </si>
+  <si>
+    <t>Power BI</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>DAX</t>
+  </si>
+  <si>
+    <t>Microsoft Excel</t>
+  </si>
+  <si>
+    <t>Decision Support</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
     <t>date_start</t>
   </si>
   <si>
@@ -41,24 +74,93 @@
     <t>location</t>
   </si>
   <si>
+    <t>Statistical Inference</t>
+  </si>
+  <si>
+    <t>Databases</t>
+  </si>
+  <si>
+    <t>Time Management</t>
+  </si>
+  <si>
+    <t>Process Excellence</t>
+  </si>
+  <si>
+    <t>GTDÂ®</t>
+  </si>
+  <si>
+    <t>Gamification</t>
+  </si>
+  <si>
+    <t>Microsoft Access</t>
+  </si>
+  <si>
+    <t>Process Improvement</t>
+  </si>
+  <si>
+    <t>Microsoft SQL Server</t>
+  </si>
+  <si>
+    <t>PowerPivot</t>
+  </si>
+  <si>
+    <t>Power Query</t>
+  </si>
+  <si>
+    <t>Operations Management</t>
+  </si>
+  <si>
+    <t>Project Planning</t>
+  </si>
+  <si>
+    <t>Logistics</t>
+  </si>
+  <si>
+    <t>Event Management</t>
+  </si>
+  <si>
     <t>Warehouse Coordinator</t>
   </si>
   <si>
+    <t>Management</t>
+  </si>
+  <si>
     <t>McDonald's</t>
   </si>
   <si>
     <t>Part-time</t>
   </si>
   <si>
+    <t>Business Process Improvement</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>RStudio</t>
+  </si>
+  <si>
     <t>Continuous</t>
   </si>
   <si>
+    <t>Microsoft Azure</t>
+  </si>
+  <si>
     <t>Operations</t>
   </si>
   <si>
+    <t>Data Visualization</t>
+  </si>
+  <si>
     <t>Kyiv, Ukraine</t>
   </si>
   <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
     <t>Operations Coordinator</t>
   </si>
   <si>
@@ -68,25 +170,61 @@
     <t>Full-time</t>
   </si>
   <si>
+    <t>Mathematics</t>
+  </si>
+  <si>
+    <t>Calculus</t>
+  </si>
+  <si>
+    <t>Economics</t>
+  </si>
+  <si>
+    <t>Data Analysis</t>
+  </si>
+  <si>
     <t>International Move Manager</t>
   </si>
   <si>
+    <t>Productivity Coaching</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Predictive Analytics</t>
+  </si>
+  <si>
+    <t>Forecasting</t>
+  </si>
+  <si>
     <t>Team Logistics Coordinator</t>
   </si>
   <si>
     <t>UEFA</t>
   </si>
   <si>
+    <t>Business Analysis</t>
+  </si>
+  <si>
     <t>Interim Contract</t>
   </si>
   <si>
+    <t>Data Modeling</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>Consulting</t>
+  </si>
+  <si>
     <t>Event Logistics Consultant</t>
   </si>
   <si>
     <t>Rock-It Cargo</t>
   </si>
   <si>
-    <t>Consulting</t>
+    <t>Business Strategy</t>
   </si>
   <si>
     <t>Moonlighting</t>
@@ -95,12 +233,21 @@
     <t>Remote</t>
   </si>
   <si>
+    <t>Strategic Planning</t>
+  </si>
+  <si>
+    <t>Financial Analysis</t>
+  </si>
+  <si>
     <t>Traffic Manager</t>
   </si>
   <si>
     <t>Suddath</t>
   </si>
   <si>
+    <t>Microsoft Dynamics CRM</t>
+  </si>
+  <si>
     <t>Jacksonville, FL</t>
   </si>
   <si>
@@ -126,153 +273,6 @@
   </si>
   <si>
     <t>Strategic Development Advisor</t>
-  </si>
-  <si>
-    <t>skill</t>
-  </si>
-  <si>
-    <t>Data Science</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>Business Intelligence</t>
-  </si>
-  <si>
-    <t>Power BI</t>
-  </si>
-  <si>
-    <t>SQL</t>
-  </si>
-  <si>
-    <t>Analysis</t>
-  </si>
-  <si>
-    <t>DAX</t>
-  </si>
-  <si>
-    <t>Microsoft Excel</t>
-  </si>
-  <si>
-    <t>Decision Support</t>
-  </si>
-  <si>
-    <t>Machine Learning</t>
-  </si>
-  <si>
-    <t>Statistical Inference</t>
-  </si>
-  <si>
-    <t>Databases</t>
-  </si>
-  <si>
-    <t>Time Management</t>
-  </si>
-  <si>
-    <t>Process Excellence</t>
-  </si>
-  <si>
-    <t>GTDÂ®</t>
-  </si>
-  <si>
-    <t>Gamification</t>
-  </si>
-  <si>
-    <t>Microsoft Access</t>
-  </si>
-  <si>
-    <t>Process Improvement</t>
-  </si>
-  <si>
-    <t>Microsoft SQL Server</t>
-  </si>
-  <si>
-    <t>PowerPivot</t>
-  </si>
-  <si>
-    <t>Power Query</t>
-  </si>
-  <si>
-    <t>Operations Management</t>
-  </si>
-  <si>
-    <t>Project Planning</t>
-  </si>
-  <si>
-    <t>Logistics</t>
-  </si>
-  <si>
-    <t>Event Management</t>
-  </si>
-  <si>
-    <t>Management</t>
-  </si>
-  <si>
-    <t>Business Process Improvement</t>
-  </si>
-  <si>
-    <t>Artificial Intelligence</t>
-  </si>
-  <si>
-    <t>RStudio</t>
-  </si>
-  <si>
-    <t>Microsoft Azure</t>
-  </si>
-  <si>
-    <t>Data Visualization</t>
-  </si>
-  <si>
-    <t>Automation</t>
-  </si>
-  <si>
-    <t>Statistics</t>
-  </si>
-  <si>
-    <t>Mathematics</t>
-  </si>
-  <si>
-    <t>Calculus</t>
-  </si>
-  <si>
-    <t>Economics</t>
-  </si>
-  <si>
-    <t>Data Analysis</t>
-  </si>
-  <si>
-    <t>Productivity Coaching</t>
-  </si>
-  <si>
-    <t>Training</t>
-  </si>
-  <si>
-    <t>Predictive Analytics</t>
-  </si>
-  <si>
-    <t>Forecasting</t>
-  </si>
-  <si>
-    <t>Business Analysis</t>
-  </si>
-  <si>
-    <t>Data Modeling</t>
-  </si>
-  <si>
-    <t>Computer Science</t>
-  </si>
-  <si>
-    <t>Business Strategy</t>
-  </si>
-  <si>
-    <t>Strategic Planning</t>
-  </si>
-  <si>
-    <t>Financial Analysis</t>
-  </si>
-  <si>
-    <t>Microsoft Dynamics CRM</t>
   </si>
   <si>
     <t>100 For Haiti</t>
@@ -333,11 +333,11 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -354,31 +354,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
@@ -389,22 +389,22 @@
         <v>39264.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3">
@@ -415,22 +415,22 @@
         <v>39661.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4">
@@ -441,22 +441,22 @@
         <v>40830.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5">
@@ -467,22 +467,22 @@
         <v>41104.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6">
@@ -493,22 +493,22 @@
         <v>41671.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7">
@@ -519,22 +519,22 @@
         <v>41548.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8">
@@ -545,22 +545,22 @@
         <v>41852.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9">
@@ -571,22 +571,22 @@
         <v>42278.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10">
@@ -597,25 +597,25 @@
         <v>42736.0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="H10" s="2">
         <v>41852.0</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11">
@@ -626,22 +626,22 @@
         <v>42826.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12">
@@ -650,22 +650,22 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13">
@@ -676,7 +676,7 @@
         <v>42705.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>87</v>
@@ -685,13 +685,13 @@
         <v>88</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>89</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14">
@@ -4659,261 +4659,261 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new theme + attempts to fix Atom/RSS
</commit_message>
<xml_diff>
--- a/content/page/data.xlsx
+++ b/content/page/data.xlsx
@@ -32,33 +32,165 @@
     <t>SQL</t>
   </si>
   <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>DAX</t>
+  </si>
+  <si>
+    <t>Microsoft Excel</t>
+  </si>
+  <si>
+    <t>Decision Support</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>Statistical Inference</t>
+  </si>
+  <si>
+    <t>Databases</t>
+  </si>
+  <si>
+    <t>Time Management</t>
+  </si>
+  <si>
+    <t>Process Excellence</t>
+  </si>
+  <si>
+    <t>GTDÂ®</t>
+  </si>
+  <si>
+    <t>Gamification</t>
+  </si>
+  <si>
+    <t>Microsoft Access</t>
+  </si>
+  <si>
     <t>date_start</t>
   </si>
   <si>
+    <t>Process Improvement</t>
+  </si>
+  <si>
     <t>date_end</t>
   </si>
   <si>
+    <t>Microsoft SQL Server</t>
+  </si>
+  <si>
     <t>title</t>
   </si>
   <si>
+    <t>PowerPivot</t>
+  </si>
+  <si>
     <t>company</t>
   </si>
   <si>
+    <t>Power Query</t>
+  </si>
+  <si>
     <t>emp_type</t>
   </si>
   <si>
+    <t>Operations Management</t>
+  </si>
+  <si>
     <t>emp_type2</t>
   </si>
   <si>
+    <t>Project Planning</t>
+  </si>
+  <si>
     <t>role</t>
   </si>
   <si>
     <t>connect_to</t>
   </si>
   <si>
+    <t>Logistics</t>
+  </si>
+  <si>
+    <t>Event Management</t>
+  </si>
+  <si>
     <t>location</t>
   </si>
   <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Business Process Improvement</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>RStudio</t>
+  </si>
+  <si>
+    <t>Microsoft Azure</t>
+  </si>
+  <si>
+    <t>Data Visualization</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>Mathematics</t>
+  </si>
+  <si>
+    <t>Calculus</t>
+  </si>
+  <si>
+    <t>Economics</t>
+  </si>
+  <si>
+    <t>Data Analysis</t>
+  </si>
+  <si>
+    <t>Productivity Coaching</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Predictive Analytics</t>
+  </si>
+  <si>
+    <t>Forecasting</t>
+  </si>
+  <si>
+    <t>Business Analysis</t>
+  </si>
+  <si>
+    <t>Data Modeling</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>Consulting</t>
+  </si>
+  <si>
+    <t>Business Strategy</t>
+  </si>
+  <si>
+    <t>Strategic Planning</t>
+  </si>
+  <si>
+    <t>Financial Analysis</t>
+  </si>
+  <si>
+    <t>Microsoft Dynamics CRM</t>
+  </si>
+  <si>
     <t>Warehouse Coordinator</t>
   </si>
   <si>
@@ -77,211 +209,79 @@
     <t>Kyiv, Ukraine</t>
   </si>
   <si>
-    <t>Analysis</t>
-  </si>
-  <si>
     <t>Operations Coordinator</t>
   </si>
   <si>
-    <t>DAX</t>
-  </si>
-  <si>
     <t>Move One Inc.</t>
   </si>
   <si>
-    <t>Microsoft Excel</t>
-  </si>
-  <si>
     <t>Full-time</t>
   </si>
   <si>
-    <t>Decision Support</t>
-  </si>
-  <si>
-    <t>Machine Learning</t>
-  </si>
-  <si>
     <t>International Move Manager</t>
   </si>
   <si>
-    <t>Statistical Inference</t>
-  </si>
-  <si>
-    <t>Databases</t>
-  </si>
-  <si>
-    <t>Time Management</t>
-  </si>
-  <si>
-    <t>Process Excellence</t>
-  </si>
-  <si>
     <t>Team Logistics Coordinator</t>
   </si>
   <si>
     <t>UEFA</t>
   </si>
   <si>
-    <t>GTDÂ®</t>
-  </si>
-  <si>
     <t>Interim Contract</t>
   </si>
   <si>
-    <t>Gamification</t>
-  </si>
-  <si>
-    <t>Microsoft Access</t>
-  </si>
-  <si>
     <t>Event Logistics Consultant</t>
   </si>
   <si>
-    <t>Process Improvement</t>
-  </si>
-  <si>
     <t>Rock-It Cargo</t>
   </si>
   <si>
-    <t>Consulting</t>
-  </si>
-  <si>
     <t>Moonlighting</t>
   </si>
   <si>
-    <t>Microsoft SQL Server</t>
-  </si>
-  <si>
     <t>Remote</t>
   </si>
   <si>
-    <t>PowerPivot</t>
-  </si>
-  <si>
     <t>Traffic Manager</t>
   </si>
   <si>
-    <t>Power Query</t>
-  </si>
-  <si>
     <t>Suddath</t>
   </si>
   <si>
-    <t>Operations Management</t>
-  </si>
-  <si>
-    <t>Project Planning</t>
-  </si>
-  <si>
     <t>Jacksonville, FL</t>
   </si>
   <si>
-    <t>Logistics</t>
-  </si>
-  <si>
-    <t>Event Management</t>
-  </si>
-  <si>
     <t>Jr. Analyst</t>
   </si>
   <si>
-    <t>Management</t>
-  </si>
-  <si>
-    <t>Business Process Improvement</t>
-  </si>
-  <si>
-    <t>Artificial Intelligence</t>
-  </si>
-  <si>
     <t>Analytics</t>
   </si>
   <si>
-    <t>RStudio</t>
-  </si>
-  <si>
-    <t>Microsoft Azure</t>
-  </si>
-  <si>
     <t>Dispatch</t>
   </si>
   <si>
-    <t>Data Visualization</t>
-  </si>
-  <si>
-    <t>Automation</t>
-  </si>
-  <si>
     <t>Seattle, WA</t>
   </si>
   <si>
-    <t>Statistics</t>
-  </si>
-  <si>
-    <t>Mathematics</t>
-  </si>
-  <si>
     <t>Data Analyst</t>
   </si>
   <si>
-    <t>Calculus</t>
-  </si>
-  <si>
-    <t>Economics</t>
-  </si>
-  <si>
-    <t>Data Analysis</t>
-  </si>
-  <si>
-    <t>Productivity Coaching</t>
-  </si>
-  <si>
     <t>Business Intelligence Analyst</t>
   </si>
   <si>
-    <t>Training</t>
-  </si>
-  <si>
-    <t>Predictive Analytics</t>
-  </si>
-  <si>
-    <t>Forecasting</t>
-  </si>
-  <si>
-    <t>Business Analysis</t>
-  </si>
-  <si>
     <t>Manager, Business Intelligence &amp; CRM</t>
   </si>
   <si>
-    <t>Data Modeling</t>
-  </si>
-  <si>
-    <t>Computer Science</t>
-  </si>
-  <si>
     <t>Strategic Development Advisor</t>
   </si>
   <si>
-    <t>Business Strategy</t>
-  </si>
-  <si>
     <t>100 For Haiti</t>
   </si>
   <si>
     <t>Pro bono consult.</t>
   </si>
   <si>
-    <t>Strategic Planning</t>
-  </si>
-  <si>
     <t>Leadership</t>
-  </si>
-  <si>
-    <t>Financial Analysis</t>
-  </si>
-  <si>
-    <t>Microsoft Dynamics CRM</t>
   </si>
 </sst>
 </file>
@@ -354,31 +354,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2">
@@ -389,22 +389,22 @@
         <v>39264.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3">
@@ -415,22 +415,22 @@
         <v>39661.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4">
@@ -441,22 +441,22 @@
         <v>40830.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5">
@@ -467,22 +467,22 @@
         <v>41104.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6">
@@ -493,22 +493,22 @@
         <v>41671.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7">
@@ -519,22 +519,22 @@
         <v>41548.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8">
@@ -545,22 +545,22 @@
         <v>41852.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9">
@@ -571,22 +571,22 @@
         <v>42278.0</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="I9" s="1" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10">
@@ -597,25 +597,25 @@
         <v>42736.0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="H10" s="2">
         <v>41852.0</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11">
@@ -626,22 +626,22 @@
         <v>42826.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12">
@@ -650,22 +650,22 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13">
@@ -676,22 +676,22 @@
         <v>42705.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14">
@@ -4698,222 +4698,222 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update gitignore and config.toml
</commit_message>
<xml_diff>
--- a/content/page/data.xlsx
+++ b/content/page/data.xlsx
@@ -14,6 +14,111 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="90">
   <si>
+    <t>date_start</t>
+  </si>
+  <si>
+    <t>date_end</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>emp_type</t>
+  </si>
+  <si>
+    <t>emp_type2</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>connect_to</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Warehouse Coordinator</t>
+  </si>
+  <si>
+    <t>McDonald's</t>
+  </si>
+  <si>
+    <t>Part-time</t>
+  </si>
+  <si>
+    <t>Continuous</t>
+  </si>
+  <si>
+    <t>Operations</t>
+  </si>
+  <si>
+    <t>Kyiv, Ukraine</t>
+  </si>
+  <si>
+    <t>Operations Coordinator</t>
+  </si>
+  <si>
+    <t>Move One Inc.</t>
+  </si>
+  <si>
+    <t>Full-time</t>
+  </si>
+  <si>
+    <t>International Move Manager</t>
+  </si>
+  <si>
+    <t>Team Logistics Coordinator</t>
+  </si>
+  <si>
+    <t>UEFA</t>
+  </si>
+  <si>
+    <t>Interim Contract</t>
+  </si>
+  <si>
+    <t>Event Logistics Consultant</t>
+  </si>
+  <si>
+    <t>Rock-It Cargo</t>
+  </si>
+  <si>
+    <t>Consulting</t>
+  </si>
+  <si>
+    <t>Moonlighting</t>
+  </si>
+  <si>
+    <t>Remote</t>
+  </si>
+  <si>
+    <t>Traffic Manager</t>
+  </si>
+  <si>
+    <t>Suddath</t>
+  </si>
+  <si>
+    <t>Jacksonville, FL</t>
+  </si>
+  <si>
+    <t>Jr. Analyst</t>
+  </si>
+  <si>
+    <t>Analytics</t>
+  </si>
+  <si>
+    <t>Dispatch</t>
+  </si>
+  <si>
+    <t>Seattle, WA</t>
+  </si>
+  <si>
+    <t>Data Analyst</t>
+  </si>
+  <si>
     <t>skill</t>
   </si>
   <si>
@@ -38,6 +143,9 @@
     <t>DAX</t>
   </si>
   <si>
+    <t>Business Intelligence Analyst</t>
+  </si>
+  <si>
     <t>Microsoft Excel</t>
   </si>
   <si>
@@ -50,6 +158,9 @@
     <t>Statistical Inference</t>
   </si>
   <si>
+    <t>Manager, Business Intelligence &amp; CRM</t>
+  </si>
+  <si>
     <t>Databases</t>
   </si>
   <si>
@@ -59,66 +170,51 @@
     <t>Process Excellence</t>
   </si>
   <si>
+    <t>Strategic Development Advisor</t>
+  </si>
+  <si>
+    <t>100 For Haiti</t>
+  </si>
+  <si>
     <t>GTDÂ®</t>
   </si>
   <si>
+    <t>Pro bono consult.</t>
+  </si>
+  <si>
+    <t>Leadership</t>
+  </si>
+  <si>
     <t>Gamification</t>
   </si>
   <si>
     <t>Microsoft Access</t>
   </si>
   <si>
-    <t>date_start</t>
-  </si>
-  <si>
     <t>Process Improvement</t>
   </si>
   <si>
-    <t>date_end</t>
-  </si>
-  <si>
     <t>Microsoft SQL Server</t>
   </si>
   <si>
-    <t>title</t>
-  </si>
-  <si>
     <t>PowerPivot</t>
   </si>
   <si>
-    <t>company</t>
-  </si>
-  <si>
     <t>Power Query</t>
   </si>
   <si>
-    <t>emp_type</t>
-  </si>
-  <si>
     <t>Operations Management</t>
   </si>
   <si>
-    <t>emp_type2</t>
-  </si>
-  <si>
     <t>Project Planning</t>
   </si>
   <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>connect_to</t>
-  </si>
-  <si>
     <t>Logistics</t>
   </si>
   <si>
     <t>Event Management</t>
   </si>
   <si>
-    <t>location</t>
-  </si>
-  <si>
     <t>Management</t>
   </si>
   <si>
@@ -176,9 +272,6 @@
     <t>Computer Science</t>
   </si>
   <si>
-    <t>Consulting</t>
-  </si>
-  <si>
     <t>Business Strategy</t>
   </si>
   <si>
@@ -189,99 +282,6 @@
   </si>
   <si>
     <t>Microsoft Dynamics CRM</t>
-  </si>
-  <si>
-    <t>Warehouse Coordinator</t>
-  </si>
-  <si>
-    <t>McDonald's</t>
-  </si>
-  <si>
-    <t>Part-time</t>
-  </si>
-  <si>
-    <t>Continuous</t>
-  </si>
-  <si>
-    <t>Operations</t>
-  </si>
-  <si>
-    <t>Kyiv, Ukraine</t>
-  </si>
-  <si>
-    <t>Operations Coordinator</t>
-  </si>
-  <si>
-    <t>Move One Inc.</t>
-  </si>
-  <si>
-    <t>Full-time</t>
-  </si>
-  <si>
-    <t>International Move Manager</t>
-  </si>
-  <si>
-    <t>Team Logistics Coordinator</t>
-  </si>
-  <si>
-    <t>UEFA</t>
-  </si>
-  <si>
-    <t>Interim Contract</t>
-  </si>
-  <si>
-    <t>Event Logistics Consultant</t>
-  </si>
-  <si>
-    <t>Rock-It Cargo</t>
-  </si>
-  <si>
-    <t>Moonlighting</t>
-  </si>
-  <si>
-    <t>Remote</t>
-  </si>
-  <si>
-    <t>Traffic Manager</t>
-  </si>
-  <si>
-    <t>Suddath</t>
-  </si>
-  <si>
-    <t>Jacksonville, FL</t>
-  </si>
-  <si>
-    <t>Jr. Analyst</t>
-  </si>
-  <si>
-    <t>Analytics</t>
-  </si>
-  <si>
-    <t>Dispatch</t>
-  </si>
-  <si>
-    <t>Seattle, WA</t>
-  </si>
-  <si>
-    <t>Data Analyst</t>
-  </si>
-  <si>
-    <t>Business Intelligence Analyst</t>
-  </si>
-  <si>
-    <t>Manager, Business Intelligence &amp; CRM</t>
-  </si>
-  <si>
-    <t>Strategic Development Advisor</t>
-  </si>
-  <si>
-    <t>100 For Haiti</t>
-  </si>
-  <si>
-    <t>Pro bono consult.</t>
-  </si>
-  <si>
-    <t>Leadership</t>
   </si>
 </sst>
 </file>
@@ -354,31 +354,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2">
@@ -389,22 +389,22 @@
         <v>39264.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
@@ -415,22 +415,22 @@
         <v>39661.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -441,22 +441,22 @@
         <v>40830.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
@@ -467,22 +467,22 @@
         <v>41104.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
@@ -493,22 +493,22 @@
         <v>41671.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>75</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7">
@@ -519,22 +519,22 @@
         <v>41548.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8">
@@ -545,22 +545,22 @@
         <v>41852.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9">
@@ -571,22 +571,22 @@
         <v>42278.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10">
@@ -597,25 +597,25 @@
         <v>42736.0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="H10" s="2">
         <v>41852.0</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>75</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11">
@@ -626,22 +626,22 @@
         <v>42826.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12">
@@ -650,22 +650,22 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13">
@@ -676,22 +676,22 @@
         <v>42705.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>75</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14">
@@ -4659,261 +4659,261 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix categories and add crosspost links
</commit_message>
<xml_diff>
--- a/content/page/data.xlsx
+++ b/content/page/data.xlsx
@@ -71,30 +71,177 @@
     <t>International Move Manager</t>
   </si>
   <si>
+    <t>skill</t>
+  </si>
+  <si>
+    <t>Data Science</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Business Intelligence</t>
+  </si>
+  <si>
+    <t>Power BI</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>DAX</t>
+  </si>
+  <si>
+    <t>Microsoft Excel</t>
+  </si>
+  <si>
+    <t>Decision Support</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>Statistical Inference</t>
+  </si>
+  <si>
+    <t>Databases</t>
+  </si>
+  <si>
+    <t>Time Management</t>
+  </si>
+  <si>
+    <t>Process Excellence</t>
+  </si>
+  <si>
+    <t>GTDÂ®</t>
+  </si>
+  <si>
+    <t>Gamification</t>
+  </si>
+  <si>
+    <t>Microsoft Access</t>
+  </si>
+  <si>
+    <t>Process Improvement</t>
+  </si>
+  <si>
+    <t>Microsoft SQL Server</t>
+  </si>
+  <si>
+    <t>PowerPivot</t>
+  </si>
+  <si>
+    <t>Power Query</t>
+  </si>
+  <si>
+    <t>Operations Management</t>
+  </si>
+  <si>
+    <t>Project Planning</t>
+  </si>
+  <si>
+    <t>Logistics</t>
+  </si>
+  <si>
+    <t>Event Management</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Business Process Improvement</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>RStudio</t>
+  </si>
+  <si>
+    <t>Microsoft Azure</t>
+  </si>
+  <si>
+    <t>Data Visualization</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>Mathematics</t>
+  </si>
+  <si>
+    <t>Calculus</t>
+  </si>
+  <si>
+    <t>Economics</t>
+  </si>
+  <si>
+    <t>Data Analysis</t>
+  </si>
+  <si>
+    <t>Productivity Coaching</t>
+  </si>
+  <si>
     <t>Team Logistics Coordinator</t>
   </si>
   <si>
+    <t>Training</t>
+  </si>
+  <si>
     <t>UEFA</t>
   </si>
   <si>
+    <t>Predictive Analytics</t>
+  </si>
+  <si>
     <t>Interim Contract</t>
   </si>
   <si>
+    <t>Forecasting</t>
+  </si>
+  <si>
+    <t>Business Analysis</t>
+  </si>
+  <si>
+    <t>Data Modeling</t>
+  </si>
+  <si>
     <t>Event Logistics Consultant</t>
   </si>
   <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
     <t>Rock-It Cargo</t>
   </si>
   <si>
     <t>Consulting</t>
   </si>
   <si>
+    <t>Business Strategy</t>
+  </si>
+  <si>
     <t>Moonlighting</t>
   </si>
   <si>
+    <t>Strategic Planning</t>
+  </si>
+  <si>
     <t>Remote</t>
   </si>
   <si>
+    <t>Financial Analysis</t>
+  </si>
+  <si>
+    <t>Microsoft Dynamics CRM</t>
+  </si>
+  <si>
     <t>Traffic Manager</t>
   </si>
   <si>
@@ -119,169 +266,22 @@
     <t>Data Analyst</t>
   </si>
   <si>
-    <t>skill</t>
-  </si>
-  <si>
-    <t>Data Science</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>Business Intelligence</t>
-  </si>
-  <si>
-    <t>Power BI</t>
-  </si>
-  <si>
-    <t>SQL</t>
-  </si>
-  <si>
-    <t>Analysis</t>
-  </si>
-  <si>
-    <t>DAX</t>
-  </si>
-  <si>
     <t>Business Intelligence Analyst</t>
   </si>
   <si>
-    <t>Microsoft Excel</t>
-  </si>
-  <si>
-    <t>Decision Support</t>
-  </si>
-  <si>
-    <t>Machine Learning</t>
-  </si>
-  <si>
-    <t>Statistical Inference</t>
-  </si>
-  <si>
     <t>Manager, Business Intelligence &amp; CRM</t>
   </si>
   <si>
-    <t>Databases</t>
-  </si>
-  <si>
-    <t>Time Management</t>
-  </si>
-  <si>
-    <t>Process Excellence</t>
-  </si>
-  <si>
     <t>Strategic Development Advisor</t>
   </si>
   <si>
     <t>100 For Haiti</t>
   </si>
   <si>
-    <t>GTDÂ®</t>
-  </si>
-  <si>
     <t>Pro bono consult.</t>
   </si>
   <si>
     <t>Leadership</t>
-  </si>
-  <si>
-    <t>Gamification</t>
-  </si>
-  <si>
-    <t>Microsoft Access</t>
-  </si>
-  <si>
-    <t>Process Improvement</t>
-  </si>
-  <si>
-    <t>Microsoft SQL Server</t>
-  </si>
-  <si>
-    <t>PowerPivot</t>
-  </si>
-  <si>
-    <t>Power Query</t>
-  </si>
-  <si>
-    <t>Operations Management</t>
-  </si>
-  <si>
-    <t>Project Planning</t>
-  </si>
-  <si>
-    <t>Logistics</t>
-  </si>
-  <si>
-    <t>Event Management</t>
-  </si>
-  <si>
-    <t>Management</t>
-  </si>
-  <si>
-    <t>Business Process Improvement</t>
-  </si>
-  <si>
-    <t>Artificial Intelligence</t>
-  </si>
-  <si>
-    <t>RStudio</t>
-  </si>
-  <si>
-    <t>Microsoft Azure</t>
-  </si>
-  <si>
-    <t>Data Visualization</t>
-  </si>
-  <si>
-    <t>Automation</t>
-  </si>
-  <si>
-    <t>Statistics</t>
-  </si>
-  <si>
-    <t>Mathematics</t>
-  </si>
-  <si>
-    <t>Calculus</t>
-  </si>
-  <si>
-    <t>Economics</t>
-  </si>
-  <si>
-    <t>Data Analysis</t>
-  </si>
-  <si>
-    <t>Productivity Coaching</t>
-  </si>
-  <si>
-    <t>Training</t>
-  </si>
-  <si>
-    <t>Predictive Analytics</t>
-  </si>
-  <si>
-    <t>Forecasting</t>
-  </si>
-  <si>
-    <t>Business Analysis</t>
-  </si>
-  <si>
-    <t>Data Modeling</t>
-  </si>
-  <si>
-    <t>Computer Science</t>
-  </si>
-  <si>
-    <t>Business Strategy</t>
-  </si>
-  <si>
-    <t>Strategic Planning</t>
-  </si>
-  <si>
-    <t>Financial Analysis</t>
-  </si>
-  <si>
-    <t>Microsoft Dynamics CRM</t>
   </si>
 </sst>
 </file>
@@ -467,13 +467,13 @@
         <v>41104.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>12</v>
@@ -493,22 +493,22 @@
         <v>41671.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7">
@@ -519,10 +519,10 @@
         <v>41548.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>17</v>
@@ -534,7 +534,7 @@
         <v>13</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8">
@@ -545,10 +545,10 @@
         <v>41852.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>17</v>
@@ -557,10 +557,10 @@
         <v>12</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9">
@@ -571,10 +571,10 @@
         <v>42278.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>17</v>
@@ -586,7 +586,7 @@
         <v>13</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10">
@@ -597,10 +597,10 @@
         <v>42736.0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>17</v>
@@ -609,13 +609,13 @@
         <v>12</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="H10" s="2">
         <v>41852.0</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11">
@@ -626,10 +626,10 @@
         <v>42826.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>17</v>
@@ -638,10 +638,10 @@
         <v>12</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12">
@@ -650,10 +650,10 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>17</v>
@@ -662,10 +662,10 @@
         <v>12</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13">
@@ -676,22 +676,22 @@
         <v>42705.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14">
@@ -4659,261 +4659,261 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix permalinks and gitignore
</commit_message>
<xml_diff>
--- a/content/page/data.xlsx
+++ b/content/page/data.xlsx
@@ -14,6 +14,144 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="90">
   <si>
+    <t>skill</t>
+  </si>
+  <si>
+    <t>Data Science</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Business Intelligence</t>
+  </si>
+  <si>
+    <t>Power BI</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>DAX</t>
+  </si>
+  <si>
+    <t>Microsoft Excel</t>
+  </si>
+  <si>
+    <t>Decision Support</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>Statistical Inference</t>
+  </si>
+  <si>
+    <t>Databases</t>
+  </si>
+  <si>
+    <t>Time Management</t>
+  </si>
+  <si>
+    <t>Process Excellence</t>
+  </si>
+  <si>
+    <t>GTDÂ®</t>
+  </si>
+  <si>
+    <t>Gamification</t>
+  </si>
+  <si>
+    <t>Microsoft Access</t>
+  </si>
+  <si>
+    <t>Process Improvement</t>
+  </si>
+  <si>
+    <t>Microsoft SQL Server</t>
+  </si>
+  <si>
+    <t>PowerPivot</t>
+  </si>
+  <si>
+    <t>Power Query</t>
+  </si>
+  <si>
+    <t>Operations Management</t>
+  </si>
+  <si>
+    <t>Project Planning</t>
+  </si>
+  <si>
+    <t>Logistics</t>
+  </si>
+  <si>
+    <t>Event Management</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Business Process Improvement</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>RStudio</t>
+  </si>
+  <si>
+    <t>Microsoft Azure</t>
+  </si>
+  <si>
+    <t>Data Visualization</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>Mathematics</t>
+  </si>
+  <si>
+    <t>Calculus</t>
+  </si>
+  <si>
+    <t>Economics</t>
+  </si>
+  <si>
+    <t>Data Analysis</t>
+  </si>
+  <si>
+    <t>Productivity Coaching</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Predictive Analytics</t>
+  </si>
+  <si>
+    <t>Forecasting</t>
+  </si>
+  <si>
+    <t>Business Analysis</t>
+  </si>
+  <si>
+    <t>Data Modeling</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>Consulting</t>
+  </si>
+  <si>
     <t>date_start</t>
   </si>
   <si>
@@ -38,9 +176,21 @@
     <t>connect_to</t>
   </si>
   <si>
+    <t>Business Strategy</t>
+  </si>
+  <si>
     <t>location</t>
   </si>
   <si>
+    <t>Strategic Planning</t>
+  </si>
+  <si>
+    <t>Financial Analysis</t>
+  </si>
+  <si>
+    <t>Microsoft Dynamics CRM</t>
+  </si>
+  <si>
     <t>Warehouse Coordinator</t>
   </si>
   <si>
@@ -71,175 +221,25 @@
     <t>International Move Manager</t>
   </si>
   <si>
-    <t>skill</t>
-  </si>
-  <si>
-    <t>Data Science</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>Business Intelligence</t>
-  </si>
-  <si>
-    <t>Power BI</t>
-  </si>
-  <si>
-    <t>SQL</t>
-  </si>
-  <si>
-    <t>Analysis</t>
-  </si>
-  <si>
-    <t>DAX</t>
-  </si>
-  <si>
-    <t>Microsoft Excel</t>
-  </si>
-  <si>
-    <t>Decision Support</t>
-  </si>
-  <si>
-    <t>Machine Learning</t>
-  </si>
-  <si>
-    <t>Statistical Inference</t>
-  </si>
-  <si>
-    <t>Databases</t>
-  </si>
-  <si>
-    <t>Time Management</t>
-  </si>
-  <si>
-    <t>Process Excellence</t>
-  </si>
-  <si>
-    <t>GTDÂ®</t>
-  </si>
-  <si>
-    <t>Gamification</t>
-  </si>
-  <si>
-    <t>Microsoft Access</t>
-  </si>
-  <si>
-    <t>Process Improvement</t>
-  </si>
-  <si>
-    <t>Microsoft SQL Server</t>
-  </si>
-  <si>
-    <t>PowerPivot</t>
-  </si>
-  <si>
-    <t>Power Query</t>
-  </si>
-  <si>
-    <t>Operations Management</t>
-  </si>
-  <si>
-    <t>Project Planning</t>
-  </si>
-  <si>
-    <t>Logistics</t>
-  </si>
-  <si>
-    <t>Event Management</t>
-  </si>
-  <si>
-    <t>Management</t>
-  </si>
-  <si>
-    <t>Business Process Improvement</t>
-  </si>
-  <si>
-    <t>Artificial Intelligence</t>
-  </si>
-  <si>
-    <t>RStudio</t>
-  </si>
-  <si>
-    <t>Microsoft Azure</t>
-  </si>
-  <si>
-    <t>Data Visualization</t>
-  </si>
-  <si>
-    <t>Automation</t>
-  </si>
-  <si>
-    <t>Statistics</t>
-  </si>
-  <si>
-    <t>Mathematics</t>
-  </si>
-  <si>
-    <t>Calculus</t>
-  </si>
-  <si>
-    <t>Economics</t>
-  </si>
-  <si>
-    <t>Data Analysis</t>
-  </si>
-  <si>
-    <t>Productivity Coaching</t>
-  </si>
-  <si>
     <t>Team Logistics Coordinator</t>
   </si>
   <si>
-    <t>Training</t>
-  </si>
-  <si>
     <t>UEFA</t>
   </si>
   <si>
-    <t>Predictive Analytics</t>
-  </si>
-  <si>
     <t>Interim Contract</t>
   </si>
   <si>
-    <t>Forecasting</t>
-  </si>
-  <si>
-    <t>Business Analysis</t>
-  </si>
-  <si>
-    <t>Data Modeling</t>
-  </si>
-  <si>
     <t>Event Logistics Consultant</t>
   </si>
   <si>
-    <t>Computer Science</t>
-  </si>
-  <si>
     <t>Rock-It Cargo</t>
   </si>
   <si>
-    <t>Consulting</t>
-  </si>
-  <si>
-    <t>Business Strategy</t>
-  </si>
-  <si>
     <t>Moonlighting</t>
   </si>
   <si>
-    <t>Strategic Planning</t>
-  </si>
-  <si>
     <t>Remote</t>
-  </si>
-  <si>
-    <t>Financial Analysis</t>
-  </si>
-  <si>
-    <t>Microsoft Dynamics CRM</t>
   </si>
   <si>
     <t>Traffic Manager</t>
@@ -354,31 +354,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2">
@@ -389,22 +389,22 @@
         <v>39264.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3">
@@ -415,22 +415,22 @@
         <v>39661.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4">
@@ -441,22 +441,22 @@
         <v>40830.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5">
@@ -467,22 +467,22 @@
         <v>41104.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6">
@@ -493,22 +493,22 @@
         <v>41671.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7">
@@ -525,13 +525,13 @@
         <v>77</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>78</v>
@@ -551,10 +551,10 @@
         <v>77</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>80</v>
@@ -577,13 +577,13 @@
         <v>77</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>82</v>
@@ -603,10 +603,10 @@
         <v>77</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>80</v>
@@ -615,7 +615,7 @@
         <v>41852.0</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11">
@@ -632,10 +632,10 @@
         <v>77</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>80</v>
@@ -656,10 +656,10 @@
         <v>77</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>80</v>
@@ -685,13 +685,13 @@
         <v>88</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>89</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14">
@@ -4659,261 +4659,261 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>